<commit_message>
Imported temporal interval [BFO:0000038]
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -484,7 +484,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -512,7 +511,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -532,7 +530,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]; function [BFO:0000034];one-dimensional temporal region [BFO:0000038]; exists at [BFO:0000108]; occurrent [BFO:0000003]; has occurrent part [BFO:0000117]; has profile [BFO:0000119];process profile of [BFO:0000133]; independent continuant [BFO:0000004]; specifically dependent continuant [BFO:0000020]; immaterial entity [BFO:0000141]; material entity [BFO:0000040]; spatial region [BFO:0000006]</t>
+          <t>specifically dependent continuant [BFO:0000020]; one-dimensional temporal region [BFO:0000038]; spatial region [BFO:0000006]; role [BFO:0000023]; occurrent [BFO:0000003]; immaterial entity [BFO:0000141]; exists at [BFO:0000108]; process [BFO:0000015]; has profile [BFO:0000119]; object [BFO:0000030]; temporal interval [BFO:0000038]; material entity [BFO:0000040]; site [BFO:0000029]; object aggregate [BFO:0000027]; independent continuant [BFO:0000004]; process profile [BFO:0000144]; has occurrent part [BFO:0000117]; process profile of [BFO:0000133]; function [BFO:0000034]; disposition [BFO:0000016]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -540,7 +538,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -568,7 +565,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -596,7 +592,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -624,7 +619,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -652,7 +646,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -680,7 +673,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -708,7 +700,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -736,7 +727,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -796,7 +786,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -824,7 +813,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -852,7 +840,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -880,7 +867,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -908,7 +894,6 @@
           <t>minimal</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>